<commit_message>
Projects column in Excel templates and upload filters
</commit_message>
<xml_diff>
--- a/rotmic/static/uploadexample_cellcomponent.xlsx
+++ b/rotmic/static/uploadexample_cellcomponent.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="75" windowWidth="26265" windowHeight="15390" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-180" windowWidth="26265" windowHeight="13800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -63,9 +63,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Clear the example data (except Status and Type columns) before inserting your own data.</t>
-  </si>
-  <si>
     <t>Import of modified Cell entries</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>KanR</t>
   </si>
   <si>
-    <t>If left empty, names will be auto-generated from plasmid and strain names.</t>
-  </si>
-  <si>
     <t>Note that this would create an "empty" cell with KanR *genomic* marker. Markers are typically specified in vector backbones not here.</t>
   </si>
   <si>
@@ -109,13 +103,16 @@
   </si>
   <si>
     <t>E. coli / BL21DE3</t>
+  </si>
+  <si>
+    <t>Projects</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +140,13 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -182,7 +186,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -193,6 +197,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -201,6 +206,122 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1762125</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="190501"/>
+          <a:ext cx="10515600" cy="781050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Clear the example data (except Status and Strain</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>columns). </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Fields marked in </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Bold</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> are required. Rows without any value in the first column will be ignored.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Markers can be referenced by their ID or by their Name .</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Only specify genomic markers. Markers on the plasmid should not be specified again!</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>If left empty, names will be auto-generated from plasmid and strain names.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Projects are referenced by their name, separated by comma (you can only refer to projects that are already registered on the server).</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -488,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -499,155 +620,144 @@
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="36.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="36.7109375" customWidth="1"/>
+    <col min="6" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" t="s">
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
       <c r="C9" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="C11" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="C13" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="3:4">
@@ -655,7 +765,7 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="3:4">
@@ -663,7 +773,7 @@
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="3:4">
@@ -671,7 +781,7 @@
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="3:4">
@@ -679,7 +789,7 @@
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="3:4">
@@ -687,7 +797,7 @@
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="3:4">
@@ -695,7 +805,7 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="3:4">
@@ -703,7 +813,7 @@
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="3:4">
@@ -711,7 +821,7 @@
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="3:4">
@@ -719,7 +829,7 @@
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="3:4">
@@ -727,7 +837,7 @@
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="3:4">
@@ -735,7 +845,7 @@
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="3:4">
@@ -743,7 +853,7 @@
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="3:4">
@@ -751,7 +861,7 @@
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="3:4">
@@ -759,7 +869,7 @@
         <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="3:4">
@@ -767,7 +877,7 @@
         <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="3:4">
@@ -775,7 +885,7 @@
         <v>9</v>
       </c>
       <c r="D32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="3:4">
@@ -783,7 +893,7 @@
         <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="3:4">
@@ -791,7 +901,7 @@
         <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="3:4">
@@ -799,7 +909,7 @@
         <v>9</v>
       </c>
       <c r="D35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="3:4">
@@ -807,7 +917,7 @@
         <v>9</v>
       </c>
       <c r="D36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="3:4">
@@ -815,7 +925,7 @@
         <v>9</v>
       </c>
       <c r="D37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="3:4">
@@ -823,7 +933,7 @@
         <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="3:4">
@@ -831,7 +941,7 @@
         <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="3:4">
@@ -839,7 +949,7 @@
         <v>9</v>
       </c>
       <c r="D40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="3:4">
@@ -847,7 +957,7 @@
         <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="3:4">
@@ -855,7 +965,7 @@
         <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="3:4">
@@ -863,23 +973,40 @@
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4">
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4">
+      <c r="C45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C45">
       <formula1>statusChoices</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D45">
       <formula1>typeChoices</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="2400" verticalDpi="1200" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -887,7 +1014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -925,7 +1052,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L5" t="s">
         <v>13</v>
@@ -936,7 +1063,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L6" t="s">
         <v>13</v>
@@ -947,7 +1074,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L7" t="s">
         <v>13</v>
@@ -958,7 +1085,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L8" t="s">
         <v>13</v>
@@ -966,7 +1093,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="C9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L9" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
update Excel Import for author field
</commit_message>
<xml_diff>
--- a/rotmic/static/uploadexample_cellcomponent.xlsx
+++ b/rotmic/static/uploadexample_cellcomponent.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-180" windowWidth="26265" windowHeight="13800"/>
+    <workbookView xWindow="2055" yWindow="1020" windowWidth="26265" windowHeight="13800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Projects</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>raik, admin</t>
   </si>
 </sst>
 </file>
@@ -215,13 +221,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1762125</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -230,8 +236,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="190501"/>
-          <a:ext cx="10515600" cy="781050"/>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="11334750" cy="952499"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -293,6 +299,17 @@
             <a:rPr lang="en-US" sz="1100"/>
             <a:t> are required. Rows without any value in the first column will be ignored.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Authors: provide</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> one or more rotmic user names separated by comma.  Leave empty to register the user who is uploading the file as single author.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
         <a:p>
           <a:r>
@@ -609,39 +626,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" customWidth="1"/>
-    <col min="6" max="7" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="36.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="36.7109375" customWidth="1"/>
+    <col min="7" max="8" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="2"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="6" t="s">
         <v>0</v>
       </c>
@@ -651,23 +669,26 @@
       <c r="C7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -677,17 +698,17 @@
       <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
       <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -695,300 +716,303 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
         <v>21</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>23</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="C11" t="s">
         <v>9</v>
       </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="C13" t="s">
         <v>9</v>
       </c>
-      <c r="D13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="C14" t="s">
         <v>9</v>
       </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="C16" t="s">
         <v>9</v>
       </c>
-      <c r="D16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4">
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5">
       <c r="C17" t="s">
         <v>9</v>
       </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4">
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5">
       <c r="C18" t="s">
         <v>9</v>
       </c>
-      <c r="D18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4">
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5">
       <c r="C19" t="s">
         <v>9</v>
       </c>
-      <c r="D19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4">
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5">
       <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="D20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4">
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5">
       <c r="C21" t="s">
         <v>9</v>
       </c>
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4">
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5">
       <c r="C22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="3:4">
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5">
       <c r="C23" t="s">
         <v>9</v>
       </c>
-      <c r="D23" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="3:4">
+      <c r="E23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5">
       <c r="C24" t="s">
         <v>9</v>
       </c>
-      <c r="D24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="3:4">
+      <c r="E24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5">
       <c r="C25" t="s">
         <v>9</v>
       </c>
-      <c r="D25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="3:4">
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5">
       <c r="C26" t="s">
         <v>9</v>
       </c>
-      <c r="D26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="3:4">
+      <c r="E26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5">
       <c r="C27" t="s">
         <v>9</v>
       </c>
-      <c r="D27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="3:4">
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5">
       <c r="C28" t="s">
         <v>9</v>
       </c>
-      <c r="D28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="3:4">
+      <c r="E28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5">
       <c r="C29" t="s">
         <v>9</v>
       </c>
-      <c r="D29" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="3:4">
+      <c r="E29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5">
       <c r="C30" t="s">
         <v>9</v>
       </c>
-      <c r="D30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="3:4">
+      <c r="E30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5">
       <c r="C31" t="s">
         <v>9</v>
       </c>
-      <c r="D31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="3:4">
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5">
       <c r="C32" t="s">
         <v>9</v>
       </c>
-      <c r="D32" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4">
+      <c r="E32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5">
       <c r="C33" t="s">
         <v>9</v>
       </c>
-      <c r="D33" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4">
+      <c r="E33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5">
       <c r="C34" t="s">
         <v>9</v>
       </c>
-      <c r="D34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4">
+      <c r="E34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5">
       <c r="C35" t="s">
         <v>9</v>
       </c>
-      <c r="D35" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="3:4">
+      <c r="E35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5">
       <c r="C36" t="s">
         <v>9</v>
       </c>
-      <c r="D36" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4">
+      <c r="E36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5">
       <c r="C37" t="s">
         <v>9</v>
       </c>
-      <c r="D37" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="3:4">
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5">
       <c r="C38" t="s">
         <v>9</v>
       </c>
-      <c r="D38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="3:4">
+      <c r="E38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5">
       <c r="C39" t="s">
         <v>9</v>
       </c>
-      <c r="D39" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="3:4">
+      <c r="E39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5">
       <c r="C40" t="s">
         <v>9</v>
       </c>
-      <c r="D40" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="3:4">
+      <c r="E40" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5">
       <c r="C41" t="s">
         <v>9</v>
       </c>
-      <c r="D41" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="3:4">
+      <c r="E41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5">
       <c r="C42" t="s">
         <v>9</v>
       </c>
-      <c r="D42" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="3:4">
+      <c r="E42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5">
       <c r="C43" t="s">
         <v>9</v>
       </c>
-      <c r="D43" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="3:4">
+      <c r="E43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5">
       <c r="C44" t="s">
         <v>9</v>
       </c>
-      <c r="D44" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="3:4">
+      <c r="E44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5">
       <c r="C45" t="s">
         <v>9</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>20</v>
       </c>
     </row>
@@ -997,7 +1021,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C45">
       <formula1>statusChoices</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D45">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E45">
       <formula1>typeChoices</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>